<commit_message>
add rspec user import excel
</commit_message>
<xml_diff>
--- a/spec/data/user_import_test_files/user.xlsx
+++ b/spec/data/user_import_test_files/user.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="123820"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9230"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="_e7_94_a8_e6_88_b7_e7_ae_a1_e7_" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="114210" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -40,33 +45,33 @@
     <t>hello3</t>
   </si>
   <si>
-    <t>性别</t>
+    <t>email</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>男</t>
+    <t>aaa1@123.com</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>女</t>
+    <t>aaa2@123.com</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>男</t>
+    <t>aaa3@123.com</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;¥&quot;* #,##0_ ;_ &quot;¥&quot;* \-#,##0_ ;_ &quot;¥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;¥&quot;* #,##0_ ;_ &quot;¥&quot;* \-#,##0_ ;_ &quot;¥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -95,6 +100,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -131,18 +143,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -157,21 +172,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Comma" xfId="1"/>
     <cellStyle name="Comma[0]" xfId="2"/>
     <cellStyle name="Currency" xfId="3"/>
     <cellStyle name="Currency[0]" xfId="4"/>
     <cellStyle name="Normal" xfId="5"/>
     <cellStyle name="Percent" xfId="6"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16"/>
@@ -459,16 +475,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.08203125" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="33.33203125" customWidth="1"/>
   </cols>
@@ -491,8 +507,8 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -502,7 +518,7 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -513,17 +529,27 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>